<commit_message>
Fixed UID gen, improved Tkinter
</commit_message>
<xml_diff>
--- a/Prices.xlsx
+++ b/Prices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vyoman\Programming\Projects\PriceScraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F7B932-196D-4D2D-8534-443928441D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1363C839-A33F-4686-9885-2E10BB50A700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{4CA0D5BF-84AC-4821-8BF7-33B18E7F3AC3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
   <si>
     <t>| Timestamp           | UID   | Name                                                                                                         | Price  |</t>
   </si>
@@ -100,6 +100,87 @@
   </si>
   <si>
     <t>| 2023-01-22 10:25:29 | P006A | Samsung Galaxy S22 Ultra 5G (Phantom Black, 12GB, 256GB Storage) with No Cost EMI/Additional Exchange Offers | 106999 |</t>
+  </si>
+  <si>
+    <t>+---------------------+-------+-----------------------------------------+--------+</t>
+  </si>
+  <si>
+    <t>| Timestamp           | UID   | Name                                    | Price  |</t>
+  </si>
+  <si>
+    <t>| 2023-01-22 12:16:59 | P001F | APPLE iPhone 14 (Blue, 128 GB)          |  72999 |</t>
+  </si>
+  <si>
+    <t>| 2023-01-22 12:16:59 | P002F | Xbox Series S Console 512 GB  (White)   |  30490 |</t>
+  </si>
+  <si>
+    <t>| 2023-01-22 12:18:14 | P001A | Apple iPhone 14 Pro Max 1TB Space Black | 182999 |</t>
+  </si>
+  <si>
+    <t>| 2023-01-22 12:18:17 | P002A | Apple iPhone 13 (128GB) - Pink          |  61999 |</t>
+  </si>
+  <si>
+    <t>| 2023-01-22 12:18:18 | P001F | APPLE iPhone 14 (Blue, 128 GB)          |  72999 |</t>
+  </si>
+  <si>
+    <t>| 2023-01-22 12:18:19 | P002F | Xbox Series S Console 512 GB  (White)   |  30490 |</t>
+  </si>
+  <si>
+    <t>| 2023-01-22 12:40:35 | P001A | Apple iPhone 14 Pro Max 1TB Space Black | 182999 |</t>
+  </si>
+  <si>
+    <t>| 2023-01-22 12:40:38 | P002A | Apple iPhone 13 (128GB) - Pink          |  61999 |</t>
+  </si>
+  <si>
+    <t>| 2023-01-22 12:40:39 | P001F | APPLE iPhone 14 (Blue, 128 GB)          |  72999 |</t>
+  </si>
+  <si>
+    <t>| 2023-01-22 12:40:39 | P002F | Xbox Series S Console 512 GB  (White)   |  30490 |</t>
+  </si>
+  <si>
+    <t>| 2023-01-22 12:45:09 | P001A | Apple iPhone 14 Pro Max 1TB Space Black | 182999 |</t>
+  </si>
+  <si>
+    <t>| 2023-01-22 12:45:12 | P002A | Apple iPhone 13 (128GB) - Pink          |  61999 |</t>
+  </si>
+  <si>
+    <t>| 2023-01-22 12:45:13 | P001F | APPLE iPhone 14 (Blue, 128 GB)          |  72999 |</t>
+  </si>
+  <si>
+    <t>| 2023-01-22 12:45:13 | P002F | Xbox Series S Console 512 GB  (White)   |  30490 |</t>
+  </si>
+  <si>
+    <t>| 2023-01-22 12:48:26 | P001A | Apple iPhone 14 Pro Max 1TB Space Black | 182999 |</t>
+  </si>
+  <si>
+    <t>| 2023-01-22 12:48:29 | P002A | Apple iPhone 13 (128GB) - Pink          |  61999 |</t>
+  </si>
+  <si>
+    <t>| 2023-01-22 12:48:30 | P001F | APPLE iPhone 14 (Blue, 128 GB)          |  72999 |</t>
+  </si>
+  <si>
+    <t>| 2023-01-22 12:48:31 | P002F | Xbox Series S Console 512 GB  (White)   |  30490 |</t>
+  </si>
+  <si>
+    <t>| 2023-01-22 12:54:45 | P001A | Apple iPhone 14 Pro Max 1TB Space Black | 182999 |</t>
+  </si>
+  <si>
+    <t>| 2023-01-22 12:54:48 | P002A | Apple iPhone 13 (128GB) - Pink          |  61999 |</t>
+  </si>
+  <si>
+    <t>| 2023-01-22 12:54:48 | P001F | APPLE iPhone 14 (Blue, 128 GB)          |  72999 |</t>
+  </si>
+  <si>
+    <t>| 2023-01-22 12:54:49 | P002F | Xbox Series S Console 512 GB  (White)   |  30490 |</t>
+  </si>
+  <si>
+    <t>| 2023-01-22 13:00:56 | P002A | Apple iPhone 13 (128GB) - Pink          |  61999 |</t>
+  </si>
+  <si>
+    <t>| 2023-01-22 13:00:57 | P001F | APPLE iPhone 14 (Blue, 128 GB)          |  72999 |</t>
+  </si>
+  <si>
+    <t>| 2023-01-22 13:00:58 | P002F | Xbox Series S Console 512 GB  (White)   |  30490 |</t>
   </si>
 </sst>
 </file>
@@ -451,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1516DCC9-10CE-4E95-990B-FC69521D155A}">
-  <dimension ref="A1:A29"/>
+  <dimension ref="A1:A59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:A29"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -604,6 +685,151 @@
         <v>1</v>
       </c>
     </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A54" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>